<commit_message>
plotting updates and corrections
Minor changes to figure size and visible/invisible features made during replotting process for editorial revisions using .svg format. Error corrected in 4-14-2023 plating data and subsequent transcription into Isolate DA plating summary and use in Figure 5E. Isolate DA plating summary updated with all replicate data for reanalysis and replotting for Figure 5E.
</commit_message>
<xml_diff>
--- a/Experiments/Figure 5E/4-15 2023 2744 2430 plating/4-14-2023 Plating.xlsx
+++ b/Experiments/Figure 5E/4-15 2023 2744 2430 plating/4-14-2023 Plating.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Helena\Documents\Helena\Duke\You Lab\Projects\Dosing Project\Experiments\2023 Population Composition\4-15 2023 2744 2430 plating\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Helena\Documents\GitHub\combination-antibiotic-selection\Experiments\Figure 5E\4-15 2023 2744 2430 plating\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF642AF-4FA8-4E3C-BCD9-427FD4552416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7556B8EB-8DD7-4120-BF81-E3BBFA84F2A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{913E35F3-A054-4690-A30A-1DF2F3FCA5B8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{913E35F3-A054-4690-A30A-1DF2F3FCA5B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Plating" sheetId="2" r:id="rId1"/>
@@ -29,8 +29,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -205,10 +203,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -5987,41 +5985,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C8D8809-5B56-47EF-993F-36560E82ED92}">
   <dimension ref="A1:AS99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G59" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y72" activeCellId="1" sqref="Y69 Y72"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AA63" sqref="AA63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="9" width="11.5546875" style="2" customWidth="1"/>
-    <col min="10" max="13" width="9.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="9.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="11.54296875" style="2" customWidth="1"/>
+    <col min="10" max="13" width="9.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.90625" style="2"/>
     <col min="15" max="15" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="12.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.88671875" style="2"/>
-    <col min="22" max="22" width="13.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.21875" style="2" customWidth="1"/>
-    <col min="24" max="24" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="14.6640625" style="2" customWidth="1"/>
-    <col min="27" max="28" width="9.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="12.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.90625" style="2"/>
+    <col min="22" max="22" width="13.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.1796875" style="2" customWidth="1"/>
+    <col min="24" max="24" width="14.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="14.6328125" style="2" customWidth="1"/>
+    <col min="27" max="28" width="9.1796875" style="2" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="11" style="2" bestFit="1" customWidth="1"/>
     <col min="30" max="32" width="11" style="2" customWidth="1"/>
-    <col min="33" max="34" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="36" max="38" width="8.88671875" style="2"/>
-    <col min="39" max="39" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="40" max="43" width="9.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="13.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="36" max="38" width="8.90625" style="2"/>
+    <col min="39" max="39" width="13.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="40" max="43" width="9.08984375" style="2" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="45" max="16384" width="8.88671875" style="2"/>
+    <col min="45" max="16384" width="8.90625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -6077,7 +6075,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -6186,7 +6184,7 @@
         <v>1.9230769230769232E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>0</v>
       </c>
@@ -6320,7 +6318,7 @@
         <v>0.99986516853932583</v>
       </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>0</v>
       </c>
@@ -6421,7 +6419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>0</v>
       </c>
@@ -6522,7 +6520,7 @@
         <v>0.49844236760124611</v>
       </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>0</v>
       </c>
@@ -6635,7 +6633,7 @@
         <v>0.52647975077881626</v>
       </c>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>0</v>
       </c>
@@ -6736,7 +6734,7 @@
         <v>0.30703259005145794</v>
       </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>0</v>
       </c>
@@ -6825,19 +6823,19 @@
       <c r="AG8" s="2">
         <v>1600000000</v>
       </c>
-      <c r="AH8" s="2">
-        <v>970000000</v>
+      <c r="AH8" s="4">
+        <v>1333333333.3333333</v>
       </c>
       <c r="AI8" s="2">
         <f t="shared" si="0"/>
-        <v>0.39374999999999999</v>
+        <v>0.16666666666666671</v>
       </c>
       <c r="AJ8" s="2">
         <f t="shared" si="1"/>
-        <v>0.60624999999999996</v>
+        <v>0.83333333333333326</v>
       </c>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>0</v>
       </c>
@@ -6938,19 +6936,19 @@
       <c r="AG9" s="2">
         <v>1510000000</v>
       </c>
-      <c r="AH9" s="2">
-        <v>860000000</v>
+      <c r="AH9" s="4">
+        <v>1223333333.3333333</v>
       </c>
       <c r="AI9" s="2">
         <f t="shared" si="0"/>
-        <v>0.43046357615894038</v>
+        <v>0.18984547461368659</v>
       </c>
       <c r="AJ9" s="2">
         <f t="shared" si="1"/>
-        <v>0.56953642384105962</v>
+        <v>0.81015452538631338</v>
       </c>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>0</v>
       </c>
@@ -7051,7 +7049,7 @@
         <v>0.90543735224586297</v>
       </c>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>0</v>
       </c>
@@ -7152,7 +7150,7 @@
         <v>0.98076923076923073</v>
       </c>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>0</v>
       </c>
@@ -7265,7 +7263,7 @@
         <v>0.53643724696356276</v>
       </c>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>0</v>
       </c>
@@ -7366,7 +7364,7 @@
         <v>0.9731182795698925</v>
       </c>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>0</v>
       </c>
@@ -7467,7 +7465,7 @@
         <v>0.8382642998027614</v>
       </c>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>0</v>
       </c>
@@ -7580,7 +7578,7 @@
         <v>2.6463104325699743E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>0</v>
       </c>
@@ -7681,7 +7679,7 @@
         <v>1.3483146067415732E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>0</v>
       </c>
@@ -7750,7 +7748,7 @@
         <v>1083333333.3333333</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>24</v>
       </c>
@@ -7831,7 +7829,7 @@
         <v>124409717.37681015</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>24</v>
       </c>
@@ -7900,7 +7898,7 @@
         <v>2536666666.6666665</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>24</v>
       </c>
@@ -7969,7 +7967,7 @@
         <v>7875000000</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>24</v>
       </c>
@@ -8050,7 +8048,7 @@
         <v>70945988.845975876</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>24</v>
       </c>
@@ -8119,7 +8117,7 @@
         <v>1946666666.6666667</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>24</v>
       </c>
@@ -8188,7 +8186,7 @@
         <v>1250000000</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>24</v>
       </c>
@@ -8269,7 +8267,7 @@
         <v>30000000</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -8338,7 +8336,7 @@
         <v>2050000000</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -8407,7 +8405,7 @@
         <v>2813333333.3333335</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>24</v>
       </c>
@@ -8488,7 +8486,7 @@
         <v>50332229.56847167</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>24</v>
       </c>
@@ -8557,7 +8555,7 @@
         <v>1803333333.3333333</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>24</v>
       </c>
@@ -8626,7 +8624,7 @@
         <v>2056666666.6666667</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>24</v>
       </c>
@@ -8707,7 +8705,7 @@
         <v>65064070.986477122</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>24</v>
       </c>
@@ -8776,7 +8774,7 @@
         <v>1756666666.6666667</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>24</v>
       </c>
@@ -8845,7 +8843,7 @@
         <v>1190000000</v>
       </c>
     </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>24</v>
       </c>
@@ -8926,7 +8924,7 @@
         <v>26034165.586355515</v>
       </c>
     </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>24</v>
       </c>
@@ -8996,7 +8994,7 @@
       </c>
       <c r="AC34" s="3"/>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>24</v>
       </c>
@@ -9065,7 +9063,7 @@
         <v>2183333333.3333335</v>
       </c>
     </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>24</v>
       </c>
@@ -9146,7 +9144,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>24</v>
       </c>
@@ -9215,7 +9213,7 @@
         <v>1775000000</v>
       </c>
     </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>24</v>
       </c>
@@ -9284,7 +9282,7 @@
         <v>1410000000</v>
       </c>
     </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>24</v>
       </c>
@@ -9365,7 +9363,7 @@
         <v>30550504.633038934</v>
       </c>
     </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>24</v>
       </c>
@@ -9434,7 +9432,7 @@
         <v>3090000000</v>
       </c>
     </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>24</v>
       </c>
@@ -9503,7 +9501,7 @@
         <v>1750000000</v>
       </c>
     </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>24</v>
       </c>
@@ -9584,7 +9582,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>24</v>
       </c>
@@ -9654,7 +9652,7 @@
       </c>
       <c r="AC43" s="3"/>
     </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>24</v>
       </c>
@@ -9723,7 +9721,7 @@
         <v>1715000000</v>
       </c>
     </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>24</v>
       </c>
@@ -9806,7 +9804,7 @@
       <c r="AE45" s="3"/>
       <c r="AF45" s="3"/>
     </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>24</v>
       </c>
@@ -9875,7 +9873,7 @@
         <v>1546666666.6666667</v>
       </c>
     </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>24</v>
       </c>
@@ -9944,12 +9942,12 @@
         <v>2136666666.6666667</v>
       </c>
     </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>1</v>
       </c>
@@ -10005,7 +10003,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>0</v>
       </c>
@@ -10086,7 +10084,7 @@
         <v>17320508.075688776</v>
       </c>
     </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>0</v>
       </c>
@@ -10155,7 +10153,7 @@
         <v>920000000</v>
       </c>
     </row>
-    <row r="53" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
         <v>0</v>
       </c>
@@ -10224,7 +10222,7 @@
         <v>956666666.66666663</v>
       </c>
     </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A54" s="2">
         <v>0</v>
       </c>
@@ -10303,7 +10301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
         <v>0</v>
       </c>
@@ -10371,7 +10369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>0</v>
       </c>
@@ -10440,7 +10438,7 @@
       </c>
       <c r="AD56" s="3"/>
     </row>
-    <row r="57" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>0</v>
       </c>
@@ -10519,7 +10517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
         <v>0</v>
       </c>
@@ -10587,7 +10585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
         <v>0</v>
       </c>
@@ -10655,7 +10653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A60" s="2">
         <v>0</v>
       </c>
@@ -10736,7 +10734,7 @@
         <v>73560254.969046324</v>
       </c>
     </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A61" s="2">
         <v>0</v>
       </c>
@@ -10805,7 +10803,7 @@
         <v>525000000</v>
       </c>
     </row>
-    <row r="62" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A62" s="2">
         <v>0</v>
       </c>
@@ -10874,7 +10872,7 @@
         <v>690000000</v>
       </c>
     </row>
-    <row r="63" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A63" s="2">
         <v>0</v>
       </c>
@@ -10955,7 +10953,7 @@
         <v>48419463.487779766</v>
       </c>
     </row>
-    <row r="64" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A64" s="2">
         <v>0</v>
       </c>
@@ -11024,7 +11022,7 @@
         <v>880000000</v>
       </c>
     </row>
-    <row r="65" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A65" s="2">
         <v>0</v>
       </c>
@@ -11093,7 +11091,7 @@
         <v>455000000</v>
       </c>
     </row>
-    <row r="66" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A66" s="2">
         <v>24</v>
       </c>
@@ -11174,7 +11172,7 @@
         <v>196751394.17831609</v>
       </c>
     </row>
-    <row r="67" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A67" s="2">
         <v>24</v>
       </c>
@@ -11243,7 +11241,7 @@
         <v>895000000</v>
       </c>
     </row>
-    <row r="68" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A68" s="2">
         <v>24</v>
       </c>
@@ -11312,7 +11310,7 @@
         <v>405000000</v>
       </c>
     </row>
-    <row r="69" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A69" s="2">
         <v>24</v>
       </c>
@@ -11340,7 +11338,7 @@
       <c r="I69" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J69" s="5">
+      <c r="J69">
         <v>121</v>
       </c>
       <c r="K69" s="2">
@@ -11384,7 +11382,7 @@
         <f>AVERAGEIF(O69:T71, "&gt;0")</f>
         <v>1966666666.6666667</v>
       </c>
-      <c r="X69" s="2">
+      <c r="X69" s="4">
         <f>AVERAGE(Q69:Q71)</f>
         <v>1333333333.3333333</v>
       </c>
@@ -11393,7 +11391,7 @@
         <v>66916199.666282438</v>
       </c>
     </row>
-    <row r="70" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A70" s="2">
         <v>24</v>
       </c>
@@ -11462,7 +11460,7 @@
         <v>2583333333.3333335</v>
       </c>
     </row>
-    <row r="71" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A71" s="2">
         <v>24</v>
       </c>
@@ -11533,7 +11531,7 @@
       <c r="AD71" s="3"/>
       <c r="AF71" s="3"/>
     </row>
-    <row r="72" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A72" s="2">
         <v>24</v>
       </c>
@@ -11605,7 +11603,7 @@
         <f>AVERAGEIF(O72:T74, "&gt;0")</f>
         <v>2263333333.3333335</v>
       </c>
-      <c r="X72" s="2">
+      <c r="X72" s="4">
         <f>AVERAGE(Q72:Q74)</f>
         <v>1223333333.3333333</v>
       </c>
@@ -11614,7 +11612,7 @@
         <v>46666666.666666672</v>
       </c>
     </row>
-    <row r="73" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A73" s="2">
         <v>24</v>
       </c>
@@ -11683,7 +11681,7 @@
         <v>1155000000</v>
       </c>
     </row>
-    <row r="74" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A74" s="2">
         <v>24</v>
       </c>
@@ -11711,7 +11709,7 @@
       <c r="I74" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J74" s="5">
+      <c r="J74">
         <v>121</v>
       </c>
       <c r="K74" s="2">
@@ -11752,7 +11750,7 @@
         <v>1570000000</v>
       </c>
     </row>
-    <row r="75" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A75" s="2">
         <v>24</v>
       </c>
@@ -11833,7 +11831,7 @@
         <v>18559214.542766742</v>
       </c>
     </row>
-    <row r="76" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A76" s="2">
         <v>24</v>
       </c>
@@ -11902,7 +11900,7 @@
         <v>1500000000</v>
       </c>
     </row>
-    <row r="77" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A77" s="2">
         <v>24</v>
       </c>
@@ -11971,7 +11969,7 @@
         <v>1430000000</v>
       </c>
     </row>
-    <row r="78" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A78" s="2">
         <v>24</v>
       </c>
@@ -12052,7 +12050,7 @@
         <v>55075705.472861022</v>
       </c>
     </row>
-    <row r="79" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A79" s="2">
         <v>24</v>
       </c>
@@ -12121,7 +12119,7 @@
         <v>1055000000</v>
       </c>
     </row>
-    <row r="80" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A80" s="2">
         <v>24</v>
       </c>
@@ -12190,7 +12188,7 @@
         <v>1043333333.3333334</v>
       </c>
     </row>
-    <row r="81" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A81" s="2">
         <v>24</v>
       </c>
@@ -12271,7 +12269,7 @@
         <v>44845413.490245707</v>
       </c>
     </row>
-    <row r="82" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A82" s="2">
         <v>24</v>
       </c>
@@ -12340,7 +12338,7 @@
         <v>880000000</v>
       </c>
     </row>
-    <row r="83" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A83" s="2">
         <v>24</v>
       </c>
@@ -12409,7 +12407,7 @@
         <v>1035000000</v>
       </c>
     </row>
-    <row r="84" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A84" s="2">
         <v>24</v>
       </c>
@@ -12491,7 +12489,7 @@
       </c>
       <c r="AE84" s="3"/>
     </row>
-    <row r="85" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A85" s="2">
         <v>24</v>
       </c>
@@ -12560,7 +12558,7 @@
         <v>1120000000</v>
       </c>
     </row>
-    <row r="86" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A86" s="2">
         <v>24</v>
       </c>
@@ -12629,7 +12627,7 @@
         <v>3682500000</v>
       </c>
     </row>
-    <row r="87" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A87" s="2">
         <v>24</v>
       </c>
@@ -12710,7 +12708,7 @@
         <v>23333333.333333336</v>
       </c>
     </row>
-    <row r="88" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A88" s="2">
         <v>24</v>
       </c>
@@ -12779,7 +12777,7 @@
         <v>1390000000</v>
       </c>
     </row>
-    <row r="89" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A89" s="2">
         <v>24</v>
       </c>
@@ -12848,7 +12846,7 @@
         <v>1380000000</v>
       </c>
     </row>
-    <row r="90" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A90" s="2">
         <v>24</v>
       </c>
@@ -12929,7 +12927,7 @@
         <v>881917.10368819686</v>
       </c>
     </row>
-    <row r="91" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A91" s="2">
         <v>24</v>
       </c>
@@ -12998,7 +12996,7 @@
         <v>26500000</v>
       </c>
     </row>
-    <row r="92" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A92" s="2">
         <v>24</v>
       </c>
@@ -13067,7 +13065,7 @@
         <v>43000000</v>
       </c>
     </row>
-    <row r="93" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A93" s="2">
         <v>24</v>
       </c>
@@ -13148,7 +13146,7 @@
         <v>57735.026918962583</v>
       </c>
     </row>
-    <row r="94" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A94" s="2">
         <v>24</v>
       </c>
@@ -13217,7 +13215,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="95" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A95" s="2">
         <v>24</v>
       </c>
@@ -13286,7 +13284,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="99" spans="31:31" x14ac:dyDescent="0.3">
+    <row r="99" spans="31:31" x14ac:dyDescent="0.35">
       <c r="AE99" s="3"/>
     </row>
   </sheetData>
@@ -13305,25 +13303,25 @@
       <selection activeCell="W28" sqref="W28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="H1" s="4" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="H1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
         <v>24</v>
       </c>
@@ -13356,7 +13354,7 @@
       </c>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -13391,12 +13389,12 @@
         <v>1.31499994546175</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -13419,7 +13417,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>2620</v>
       </c>
@@ -13440,7 +13438,7 @@
         <v>1.6319999471306801</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>4682</v>
       </c>
@@ -13479,14 +13477,14 @@
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -13518,7 +13516,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>24</v>
       </c>
@@ -13533,7 +13531,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>24</v>
       </c>
@@ -13548,7 +13546,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>24</v>
       </c>
@@ -13563,7 +13561,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>24</v>
       </c>
@@ -13578,7 +13576,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>24</v>
       </c>
@@ -13593,7 +13591,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>24</v>
       </c>
@@ -13608,7 +13606,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>24</v>
       </c>
@@ -13623,7 +13621,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>24</v>
       </c>
@@ -13638,7 +13636,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>24</v>
       </c>
@@ -13653,7 +13651,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>24</v>
       </c>

</xml_diff>